<commit_message>
Update test program to handle FHIR output
</commit_message>
<xml_diff>
--- a/source_data/protocols/CDISC_Pilot_M11/CDISC_Pilot_Study_M11.xlsx
+++ b/source_data/protocols/CDISC_Pilot_M11/CDISC_Pilot_Study_M11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/CDISC_Pilot_M11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488A34F5-E525-074A-8145-AD286602EFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27260EE-6A03-C146-B2BD-F6B0FED3B467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22240" yWindow="500" windowWidth="40760" windowHeight="27240" firstSheet="14" activeTab="23" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -5833,7 +5833,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6019,6 +6019,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -10748,15 +10751,15 @@
   <dimension ref="A1:D155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="61" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" style="61" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" style="61" customWidth="1"/>
-    <col min="3" max="3" width="81.5" style="61" customWidth="1"/>
-    <col min="4" max="4" width="84.5" style="61" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" style="66" customWidth="1"/>
+    <col min="4" max="4" width="109.83203125" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -10773,12 +10776,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
         <v>877</v>
       </c>
       <c r="B2" s="11"/>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="46" t="s">
         <v>878</v>
       </c>
       <c r="D2" s="46"/>
@@ -10829,7 +10832,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="46" t="s">
         <v>887</v>
       </c>

</xml_diff>